<commit_message>
can ingest messages spreadsheet
</commit_message>
<xml_diff>
--- a/ingestion/messages.xlsx
+++ b/ingestion/messages.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardgannon/dev/go-sns/ingestion/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37B355AD-D265-844A-BD64-C65430AD30D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5945AC38-3304-1947-950C-FED64DDC3F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2680" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="69380" yWindow="5860" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="messages" sheetId="1" r:id="rId1"/>
@@ -25,28 +25,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="5" uniqueCount="5">
-  <si>
-    <t>code	subject	body</t>
-  </si>
-  <si>
-    <t>st	go-sns started	go-sns has started successfully</t>
-  </si>
-  <si>
-    <t>sh	A system is shutting down	The attached system is attempting to shutdown</t>
-  </si>
-  <si>
-    <t>tc	Task Complete	A task has been completed</t>
-  </si>
-  <si>
-    <t>tf	Task Failed	A task has failed</t>
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="15" uniqueCount="15">
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>body</t>
+  </si>
+  <si>
+    <t>st</t>
+  </si>
+  <si>
+    <t>go-sns has started successfully</t>
+  </si>
+  <si>
+    <t>The attached system is attempting to shutdown</t>
+  </si>
+  <si>
+    <t>go-sns started</t>
+  </si>
+  <si>
+    <t>sh</t>
+  </si>
+  <si>
+    <t>A system is shutting down</t>
+  </si>
+  <si>
+    <t>tc</t>
+  </si>
+  <si>
+    <t>Task Complete</t>
+  </si>
+  <si>
+    <t>A task has been completed</t>
+  </si>
+  <si>
+    <t>tf</t>
+  </si>
+  <si>
+    <t>Task Failed</t>
+  </si>
+  <si>
+    <t>A task has failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,6 +210,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -523,8 +559,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -879,36 +916,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>1</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>